<commit_message>
Correction type pour génération à partir fsh ea4a6f04ed193a83290686b2f69a3f9cd2e7f4ad
</commit_message>
<xml_diff>
--- a/poc-professionnel/ig/StructureDefinition-BoiteLettreMSS.xlsx
+++ b/poc-professionnel/ig/StructureDefinition-BoiteLettreMSS.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-17T14:35:50+00:00</t>
+    <t>2025-07-18T06:40:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -234,7 +234,7 @@
     <t>*</t>
   </si>
   <si>
-    <t xml:space="preserve">Element
+    <t xml:space="preserve">
 </t>
   </si>
   <si>
@@ -250,7 +250,7 @@
     <t>1</t>
   </si>
   <si>
-    <t xml:space="preserve">https://interop.esante.gouv.fr/ig/fhir/mos/StructureDefinition/Telecommunication
+    <t xml:space="preserve">ContactPoint {https://interop.esante.gouv.fr/ig/fhir/mos/StructureDefinition/Telecommunication}
 </t>
   </si>
   <si>
@@ -636,7 +636,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="64.53125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="77.10546875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
3e version avec organisation fichiers 79edfa974f5e8518fc0ba7f491a5a364eece9d5d
</commit_message>
<xml_diff>
--- a/poc-professionnel/ig/StructureDefinition-BoiteLettreMSS.xlsx
+++ b/poc-professionnel/ig/StructureDefinition-BoiteLettreMSS.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-18T06:40:38+00:00</t>
+    <t>2025-07-21T11:52:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -250,7 +250,7 @@
     <t>1</t>
   </si>
   <si>
-    <t xml:space="preserve">ContactPoint {https://interop.esante.gouv.fr/ig/fhir/mos/StructureDefinition/Telecommunication}
+    <t xml:space="preserve">https://interop.esante.gouv.fr/ig/fhir/mos/StructureDefinition/Telecommunication
 </t>
   </si>
   <si>
@@ -270,7 +270,7 @@
     <t>preferred</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/mos/ValueSet/TypeBAL-vs</t>
+    <t>https://interop.esante.gouv.fr/terminologies/CodeSystem-TRE-R257-TypeBAL?vs</t>
   </si>
   <si>
     <t>BoiteLettreMSS.description</t>
@@ -636,7 +636,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="77.10546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="64.53125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -651,7 +651,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="50.30859375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="64.0859375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>

</xml_diff>